<commit_message>
fix aim col bug
</commit_message>
<xml_diff>
--- a/task_table.xlsx
+++ b/task_table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PycharmProjects\pond_reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\pondo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21390" yWindow="0" windowWidth="17190" windowHeight="6195"/>
+    <workbookView xWindow="22290" yWindow="0" windowWidth="17190" windowHeight="6200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,26 +543,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="6" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.625" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.36328125" customWidth="1"/>
+    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +612,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1580</v>
       </c>
@@ -656,7 +656,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1580</v>
       </c>
@@ -700,7 +700,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1580</v>
       </c>
@@ -744,7 +744,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1580</v>
       </c>
@@ -788,7 +788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1580</v>
       </c>
@@ -832,7 +832,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1580</v>
       </c>
@@ -876,7 +876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1580</v>
       </c>
@@ -920,7 +920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1580</v>
       </c>
@@ -964,7 +964,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1580</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1580</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1580</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1580</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1580</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1580</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2250</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>2250</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2250</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2250</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>2250</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2250</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>2250</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2250</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2250</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2250</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>2250</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2250</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>2250</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2250</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1580</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1580</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2250</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2250</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1580</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2250</v>
       </c>

</xml_diff>